<commit_message>
generate the visibility graph
</commit_message>
<xml_diff>
--- a/Input data/Task_list.xlsx
+++ b/Input data/Task_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lichen/PycharmProjects/ACO_Example/Input data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7A6D38-0698-C344-9B35-0F1D20903DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DD8DB5-DA66-8F4D-8731-EB94AE9A88AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6160" yWindow="500" windowWidth="20080" windowHeight="17500" activeTab="1" xr2:uid="{72EC4D3E-5F86-F046-9AAF-2F56F54DDF76}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="16">
   <si>
     <t>Task ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -88,6 +88,14 @@
     <t>End node</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>speed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>unloading loading time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -97,7 +105,7 @@
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +144,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,7 +173,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -191,6 +205,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,19 +524,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0C464B-E021-9D41-8D89-770FE56B4B97}">
-  <dimension ref="A1:K141"/>
+  <dimension ref="A1:M141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="4" width="21.1640625" customWidth="1"/>
     <col min="6" max="7" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,11 +566,17 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -579,11 +604,17 @@
       <c r="I2" s="4">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="11">
+        <v>70</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -611,11 +642,17 @@
       <c r="I3" s="4">
         <v>0</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="11">
+        <v>70</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -643,11 +680,17 @@
       <c r="I4" s="4">
         <v>0</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11">
+        <v>70</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -675,9 +718,14 @@
       <c r="I5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -705,9 +753,14 @@
       <c r="I6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -735,8 +788,14 @@
       <c r="I7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -764,9 +823,14 @@
       <c r="I8" s="4">
         <v>0</v>
       </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -794,9 +858,14 @@
       <c r="I9" s="4">
         <v>0</v>
       </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -824,9 +893,14 @@
       <c r="I10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -854,9 +928,14 @@
       <c r="I11" s="4">
         <v>0</v>
       </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -884,9 +963,14 @@
       <c r="I12" s="4">
         <v>0</v>
       </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -914,8 +998,14 @@
       <c r="I13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -943,8 +1033,14 @@
       <c r="I14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="J14" s="4">
+        <v>2</v>
+      </c>
+      <c r="K14" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -972,8 +1068,14 @@
       <c r="I15" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="J15" s="4">
+        <v>2</v>
+      </c>
+      <c r="K15" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1001,8 +1103,14 @@
       <c r="I16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="4">
+        <v>2</v>
+      </c>
+      <c r="K16" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1030,8 +1138,14 @@
       <c r="I17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1059,8 +1173,14 @@
       <c r="I18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+      <c r="K18" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1088,8 +1208,14 @@
       <c r="I19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="4">
+        <v>2</v>
+      </c>
+      <c r="K19" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1117,8 +1243,14 @@
       <c r="I20" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1146,8 +1278,14 @@
       <c r="I21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="4">
+        <v>1</v>
+      </c>
+      <c r="K21" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -1175,8 +1313,14 @@
       <c r="I22" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
+      <c r="K22" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -1204,8 +1348,14 @@
       <c r="I23" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
+      <c r="K23" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -1233,8 +1383,14 @@
       <c r="I24" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="4">
+        <v>1</v>
+      </c>
+      <c r="K24" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -1262,8 +1418,14 @@
       <c r="I25" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="4">
+        <v>1</v>
+      </c>
+      <c r="K25" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -1291,8 +1453,14 @@
       <c r="I26" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="4">
+        <v>1</v>
+      </c>
+      <c r="K26" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -1320,8 +1488,14 @@
       <c r="I27" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="4">
+        <v>1</v>
+      </c>
+      <c r="K27" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="4">
         <f>A27+1</f>
         <v>26</v>
@@ -1350,8 +1524,14 @@
       <c r="I28" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="4">
+        <v>2</v>
+      </c>
+      <c r="K28" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="4">
         <f t="shared" ref="A29:A92" si="0">A28+1</f>
         <v>27</v>
@@ -1380,8 +1560,14 @@
       <c r="I29" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="4">
+        <v>2</v>
+      </c>
+      <c r="K29" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1410,8 +1596,14 @@
       <c r="I30" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="4">
+        <v>2</v>
+      </c>
+      <c r="K30" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1440,8 +1632,14 @@
       <c r="I31" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="4">
+        <v>2</v>
+      </c>
+      <c r="K31" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1470,8 +1668,14 @@
       <c r="I32" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="4">
+        <v>2</v>
+      </c>
+      <c r="K32" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1500,8 +1704,14 @@
       <c r="I33" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="4">
+        <v>2</v>
+      </c>
+      <c r="K33" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="4">
         <f>A33+1</f>
         <v>32</v>
@@ -1530,8 +1740,14 @@
       <c r="I34" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="4">
+        <v>2</v>
+      </c>
+      <c r="K34" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="4">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1560,8 +1776,14 @@
       <c r="I35" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="4">
+        <v>2</v>
+      </c>
+      <c r="K35" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1590,8 +1812,14 @@
       <c r="I36" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="4">
+        <v>2</v>
+      </c>
+      <c r="K36" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1620,8 +1848,14 @@
       <c r="I37" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="4">
+        <v>2</v>
+      </c>
+      <c r="K37" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1650,8 +1884,14 @@
       <c r="I38" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="4">
+        <v>2</v>
+      </c>
+      <c r="K38" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="4">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1680,8 +1920,14 @@
       <c r="I39" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="4">
+        <v>2</v>
+      </c>
+      <c r="K39" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1710,8 +1956,14 @@
       <c r="I40" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="4">
+        <v>1</v>
+      </c>
+      <c r="K40" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1740,8 +1992,14 @@
       <c r="I41" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="4">
+        <v>1</v>
+      </c>
+      <c r="K41" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1770,8 +2028,14 @@
       <c r="I42" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="4">
+        <v>1</v>
+      </c>
+      <c r="K42" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1800,8 +2064,14 @@
       <c r="I43" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="4">
+        <v>1</v>
+      </c>
+      <c r="K43" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1830,8 +2100,14 @@
       <c r="I44" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="4">
+        <v>1</v>
+      </c>
+      <c r="K44" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1860,8 +2136,14 @@
       <c r="I45" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="4">
+        <v>1</v>
+      </c>
+      <c r="K45" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1890,8 +2172,14 @@
       <c r="I46" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="4">
+        <v>1</v>
+      </c>
+      <c r="K46" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1920,8 +2208,14 @@
       <c r="I47" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="4">
+        <v>1</v>
+      </c>
+      <c r="K47" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1950,8 +2244,14 @@
       <c r="I48" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="4">
+        <v>1</v>
+      </c>
+      <c r="K48" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1980,8 +2280,14 @@
       <c r="I49" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="4">
+        <v>1</v>
+      </c>
+      <c r="K49" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2010,8 +2316,14 @@
       <c r="I50" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="4">
+        <v>1</v>
+      </c>
+      <c r="K50" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2040,8 +2352,14 @@
       <c r="I51" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="4">
+        <v>1</v>
+      </c>
+      <c r="K51" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2070,8 +2388,14 @@
       <c r="I52" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="4">
+        <v>1</v>
+      </c>
+      <c r="K52" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2100,8 +2424,14 @@
       <c r="I53" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="4">
+        <v>1</v>
+      </c>
+      <c r="K53" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="4">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2130,8 +2460,14 @@
       <c r="I54" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="4">
+        <v>1</v>
+      </c>
+      <c r="K54" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="4">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2160,8 +2496,14 @@
       <c r="I55" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="4">
+        <v>1</v>
+      </c>
+      <c r="K55" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="4">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2190,8 +2532,14 @@
       <c r="I56" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="4">
+        <v>1</v>
+      </c>
+      <c r="K56" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="4">
         <f>A56+1</f>
         <v>55</v>
@@ -2220,8 +2568,14 @@
       <c r="I57" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="4">
+        <v>1</v>
+      </c>
+      <c r="K57" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="4">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2250,8 +2604,14 @@
       <c r="I58" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="4">
+        <v>2</v>
+      </c>
+      <c r="K58" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="4">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2280,8 +2640,14 @@
       <c r="I59" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" s="4">
+        <v>2</v>
+      </c>
+      <c r="K59" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="4">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2310,8 +2676,14 @@
       <c r="I60" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" s="4">
+        <v>2</v>
+      </c>
+      <c r="K60" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="4">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2340,8 +2712,14 @@
       <c r="I61" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" s="4">
+        <v>2</v>
+      </c>
+      <c r="K61" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2370,8 +2748,14 @@
       <c r="I62" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" s="4">
+        <v>2</v>
+      </c>
+      <c r="K62" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="4">
         <f>A62+1</f>
         <v>61</v>
@@ -2400,8 +2784,14 @@
       <c r="I63" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" s="4">
+        <v>2</v>
+      </c>
+      <c r="K63" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="4">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2430,8 +2820,14 @@
       <c r="I64" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" s="4">
+        <v>1</v>
+      </c>
+      <c r="K64" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="4">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2460,8 +2856,14 @@
       <c r="I65" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" s="4">
+        <v>1</v>
+      </c>
+      <c r="K65" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2490,8 +2892,14 @@
       <c r="I66" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" s="4">
+        <v>1</v>
+      </c>
+      <c r="K66" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="4">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -2520,8 +2928,14 @@
       <c r="I67" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" s="4">
+        <v>2</v>
+      </c>
+      <c r="K67" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="4">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -2550,8 +2964,14 @@
       <c r="I68" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68" s="4">
+        <v>2</v>
+      </c>
+      <c r="K68" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="4">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -2580,8 +3000,14 @@
       <c r="I69" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69" s="4">
+        <v>2</v>
+      </c>
+      <c r="K69" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="4">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -2610,8 +3036,14 @@
       <c r="I70" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70" s="4">
+        <v>2</v>
+      </c>
+      <c r="K70" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="4">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -2640,8 +3072,14 @@
       <c r="I71" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71" s="4">
+        <v>2</v>
+      </c>
+      <c r="K71" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="4">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -2670,8 +3108,14 @@
       <c r="I72" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72" s="4">
+        <v>2</v>
+      </c>
+      <c r="K72" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="4">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -2700,8 +3144,14 @@
       <c r="I73" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73" s="4">
+        <v>2</v>
+      </c>
+      <c r="K73" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="4">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -2730,8 +3180,14 @@
       <c r="I74" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74" s="4">
+        <v>2</v>
+      </c>
+      <c r="K74" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="4">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -2760,8 +3216,14 @@
       <c r="I75" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75" s="4">
+        <v>2</v>
+      </c>
+      <c r="K75" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="4">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -2790,8 +3252,14 @@
       <c r="I76" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76" s="4">
+        <v>2</v>
+      </c>
+      <c r="K76" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="4">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -2820,8 +3288,14 @@
       <c r="I77" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77" s="4">
+        <v>2</v>
+      </c>
+      <c r="K77" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="4">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -2850,8 +3324,14 @@
       <c r="I78" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" s="4">
+        <v>2</v>
+      </c>
+      <c r="K78" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="4">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -2880,8 +3360,14 @@
       <c r="I79" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79" s="4">
+        <v>2</v>
+      </c>
+      <c r="K79" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="4">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -2910,8 +3396,14 @@
       <c r="I80" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" s="4">
+        <v>2</v>
+      </c>
+      <c r="K80" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="4">
         <f>A80+1</f>
         <v>79</v>
@@ -2940,8 +3432,14 @@
       <c r="I81" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" s="4">
+        <v>1</v>
+      </c>
+      <c r="K81" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="4">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -2970,8 +3468,14 @@
       <c r="I82" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" s="4">
+        <v>1</v>
+      </c>
+      <c r="K82" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="4">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -3000,8 +3504,14 @@
       <c r="I83" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" s="4">
+        <v>1</v>
+      </c>
+      <c r="K83" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="4">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -3030,8 +3540,14 @@
       <c r="I84" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" s="4">
+        <v>1</v>
+      </c>
+      <c r="K84" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="4">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -3060,8 +3576,14 @@
       <c r="I85" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" s="4">
+        <v>1</v>
+      </c>
+      <c r="K85" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="4">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -3090,8 +3612,14 @@
       <c r="I86" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" s="4">
+        <v>1</v>
+      </c>
+      <c r="K86" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="4">
         <f>A86+1</f>
         <v>85</v>
@@ -3120,8 +3648,14 @@
       <c r="I87" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" s="4">
+        <v>1</v>
+      </c>
+      <c r="K87" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="4">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -3150,8 +3684,14 @@
       <c r="I88" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" s="4">
+        <v>1</v>
+      </c>
+      <c r="K88" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" s="4">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -3180,8 +3720,14 @@
       <c r="I89" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" s="4">
+        <v>1</v>
+      </c>
+      <c r="K89" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="4">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -3210,8 +3756,14 @@
       <c r="I90" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" s="4">
+        <v>1</v>
+      </c>
+      <c r="K90" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="4">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -3240,8 +3792,14 @@
       <c r="I91" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" s="4">
+        <v>1</v>
+      </c>
+      <c r="K91" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="4">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -3270,8 +3828,14 @@
       <c r="I92" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92" s="4">
+        <v>1</v>
+      </c>
+      <c r="K92" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="4">
         <f t="shared" ref="A93" si="1">A92+1</f>
         <v>91</v>
@@ -3300,8 +3864,14 @@
       <c r="I93" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93" s="4">
+        <v>1</v>
+      </c>
+      <c r="K93" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="4">
         <f>A93+1</f>
         <v>92</v>
@@ -3330,8 +3900,14 @@
       <c r="I94" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94" s="4">
+        <v>1</v>
+      </c>
+      <c r="K94" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="4">
         <f t="shared" ref="A95:A115" si="2">A94+1</f>
         <v>93</v>
@@ -3360,8 +3936,14 @@
       <c r="I95" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95" s="4">
+        <v>1</v>
+      </c>
+      <c r="K95" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="4">
         <f t="shared" si="2"/>
         <v>94</v>
@@ -3390,8 +3972,14 @@
       <c r="I96" s="5">
         <v>59</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96" s="4">
+        <v>1</v>
+      </c>
+      <c r="K96" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="4">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -3420,8 +4008,14 @@
       <c r="I97" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97" s="4">
+        <v>1</v>
+      </c>
+      <c r="K97" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="4">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -3450,8 +4044,14 @@
       <c r="I98" s="5">
         <v>61</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98" s="4">
+        <v>1</v>
+      </c>
+      <c r="K98" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" s="4">
         <f t="shared" si="2"/>
         <v>97</v>
@@ -3480,8 +4080,14 @@
       <c r="I99" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="J99" s="4">
+        <v>2</v>
+      </c>
+      <c r="K99" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" s="4">
         <f>A99+1</f>
         <v>98</v>
@@ -3510,8 +4116,14 @@
       <c r="I100" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="J100" s="4">
+        <v>2</v>
+      </c>
+      <c r="K100" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" s="4">
         <f t="shared" si="2"/>
         <v>99</v>
@@ -3540,8 +4152,14 @@
       <c r="I101" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="J101" s="4">
+        <v>2</v>
+      </c>
+      <c r="K101" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" s="4">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -3570,8 +4188,14 @@
       <c r="I102" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="J102" s="4">
+        <v>2</v>
+      </c>
+      <c r="K102" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" s="4">
         <f t="shared" si="2"/>
         <v>101</v>
@@ -3600,8 +4224,14 @@
       <c r="I103" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:9">
+      <c r="J103" s="4">
+        <v>2</v>
+      </c>
+      <c r="K103" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" s="4">
         <f t="shared" si="2"/>
         <v>102</v>
@@ -3630,8 +4260,14 @@
       <c r="I104" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="J104" s="4">
+        <v>2</v>
+      </c>
+      <c r="K104" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="4">
         <f t="shared" si="2"/>
         <v>103</v>
@@ -3660,8 +4296,14 @@
       <c r="I105" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="J105" s="4">
+        <v>2</v>
+      </c>
+      <c r="K105" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" s="4">
         <f t="shared" si="2"/>
         <v>104</v>
@@ -3690,8 +4332,14 @@
       <c r="I106" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106" s="4">
+        <v>2</v>
+      </c>
+      <c r="K106" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" s="4">
         <f t="shared" si="2"/>
         <v>105</v>
@@ -3720,8 +4368,14 @@
       <c r="I107" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="J107" s="4">
+        <v>2</v>
+      </c>
+      <c r="K107" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="4">
         <f t="shared" si="2"/>
         <v>106</v>
@@ -3750,8 +4404,14 @@
       <c r="I108" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="J108" s="4">
+        <v>2</v>
+      </c>
+      <c r="K108" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" s="4">
         <f t="shared" si="2"/>
         <v>107</v>
@@ -3780,8 +4440,14 @@
       <c r="I109" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="J109" s="4">
+        <v>2</v>
+      </c>
+      <c r="K109" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" s="4">
         <f t="shared" si="2"/>
         <v>108</v>
@@ -3810,8 +4476,14 @@
       <c r="I110" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="J110" s="4">
+        <v>2</v>
+      </c>
+      <c r="K110" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" s="4">
         <f t="shared" si="2"/>
         <v>109</v>
@@ -3840,8 +4512,14 @@
       <c r="I111" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="J111" s="4">
+        <v>2</v>
+      </c>
+      <c r="K111" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" s="4">
         <f t="shared" si="2"/>
         <v>110</v>
@@ -3870,8 +4548,14 @@
       <c r="I112" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112" s="4">
+        <v>2</v>
+      </c>
+      <c r="K112" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" s="4">
         <f t="shared" si="2"/>
         <v>111</v>
@@ -3900,8 +4584,14 @@
       <c r="I113" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113" s="4">
+        <v>2</v>
+      </c>
+      <c r="K113" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" s="4">
         <f t="shared" si="2"/>
         <v>112</v>
@@ -3930,8 +4620,14 @@
       <c r="I114" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" s="4">
+        <v>2</v>
+      </c>
+      <c r="K114" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" s="4">
         <f t="shared" si="2"/>
         <v>113</v>
@@ -3960,8 +4656,14 @@
       <c r="I115" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115" s="4">
+        <v>2</v>
+      </c>
+      <c r="K115" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" s="4">
         <f>A115+1</f>
         <v>114</v>
@@ -3990,8 +4692,14 @@
       <c r="I116" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116" s="4">
+        <v>1</v>
+      </c>
+      <c r="K116" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" s="4">
         <f t="shared" ref="A117:A128" si="3">A116+1</f>
         <v>115</v>
@@ -4020,8 +4728,14 @@
       <c r="I117" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="J117" s="4">
+        <v>1</v>
+      </c>
+      <c r="K117" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" s="4">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -4050,8 +4764,14 @@
       <c r="I118" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="J118" s="4">
+        <v>1</v>
+      </c>
+      <c r="K118" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" s="4">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -4080,8 +4800,14 @@
       <c r="I119" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="J119" s="4">
+        <v>1</v>
+      </c>
+      <c r="K119" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" s="4">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -4110,8 +4836,14 @@
       <c r="I120" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="J120" s="4">
+        <v>1</v>
+      </c>
+      <c r="K120" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" s="4">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -4140,8 +4872,14 @@
       <c r="I121" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="J121" s="4">
+        <v>1</v>
+      </c>
+      <c r="K121" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" s="4">
         <f>A121+1</f>
         <v>120</v>
@@ -4170,8 +4908,14 @@
       <c r="I122" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="J122" s="4">
+        <v>1</v>
+      </c>
+      <c r="K122" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" s="4">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -4200,8 +4944,14 @@
       <c r="I123" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="J123" s="4">
+        <v>1</v>
+      </c>
+      <c r="K123" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" s="4">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -4230,8 +4980,14 @@
       <c r="I124" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="J124" s="4">
+        <v>1</v>
+      </c>
+      <c r="K124" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" s="4">
         <f t="shared" si="3"/>
         <v>123</v>
@@ -4260,8 +5016,14 @@
       <c r="I125" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="J125" s="4">
+        <v>1</v>
+      </c>
+      <c r="K125" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" s="4">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -4290,8 +5052,14 @@
       <c r="I126" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="J126" s="4">
+        <v>1</v>
+      </c>
+      <c r="K126" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" s="4">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -4320,8 +5088,14 @@
       <c r="I127" s="5">
         <v>97</v>
       </c>
-    </row>
-    <row r="128" spans="1:9">
+      <c r="J127" s="4">
+        <v>1</v>
+      </c>
+      <c r="K127" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" s="4">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -4350,8 +5124,14 @@
       <c r="I128" s="5">
         <v>98</v>
       </c>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="J128" s="4">
+        <v>1</v>
+      </c>
+      <c r="K128" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129" s="4">
         <f>A128+1</f>
         <v>127</v>
@@ -4380,8 +5160,14 @@
       <c r="I129" s="5">
         <v>99</v>
       </c>
-    </row>
-    <row r="130" spans="1:9">
+      <c r="J129" s="4">
+        <v>1</v>
+      </c>
+      <c r="K129" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130" s="4">
         <f t="shared" ref="A130:A141" si="4">A129+1</f>
         <v>128</v>
@@ -4410,8 +5196,14 @@
       <c r="I130" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="131" spans="1:9">
+      <c r="J130" s="4">
+        <v>1</v>
+      </c>
+      <c r="K130" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
       <c r="A131" s="4">
         <f t="shared" si="4"/>
         <v>129</v>
@@ -4440,8 +5232,14 @@
       <c r="I131" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:9">
+      <c r="J131" s="4">
+        <v>2</v>
+      </c>
+      <c r="K131" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
       <c r="A132" s="4">
         <f t="shared" si="4"/>
         <v>130</v>
@@ -4470,8 +5268,14 @@
       <c r="I132" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:9">
+      <c r="J132" s="4">
+        <v>2</v>
+      </c>
+      <c r="K132" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
       <c r="A133" s="4">
         <f t="shared" si="4"/>
         <v>131</v>
@@ -4500,8 +5304,14 @@
       <c r="I133" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:9">
+      <c r="J133" s="4">
+        <v>2</v>
+      </c>
+      <c r="K133" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134" s="4">
         <f t="shared" si="4"/>
         <v>132</v>
@@ -4530,8 +5340,14 @@
       <c r="I134" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:9">
+      <c r="J134" s="4">
+        <v>2</v>
+      </c>
+      <c r="K134" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135" s="4">
         <f>A134+1</f>
         <v>133</v>
@@ -4560,8 +5376,14 @@
       <c r="I135" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:9">
+      <c r="J135" s="4">
+        <v>2</v>
+      </c>
+      <c r="K135" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136" s="4">
         <f t="shared" si="4"/>
         <v>134</v>
@@ -4590,8 +5412,14 @@
       <c r="I136" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:9">
+      <c r="J136" s="4">
+        <v>2</v>
+      </c>
+      <c r="K136" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137" s="4">
         <f t="shared" si="4"/>
         <v>135</v>
@@ -4620,8 +5448,14 @@
       <c r="I137" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="J137" s="4">
+        <v>2</v>
+      </c>
+      <c r="K137" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" s="4">
         <f t="shared" si="4"/>
         <v>136</v>
@@ -4650,8 +5484,14 @@
       <c r="I138" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:9">
+      <c r="J138" s="4">
+        <v>2</v>
+      </c>
+      <c r="K138" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" s="4">
         <f t="shared" si="4"/>
         <v>137</v>
@@ -4680,8 +5520,14 @@
       <c r="I139" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:9">
+      <c r="J139" s="4">
+        <v>2</v>
+      </c>
+      <c r="K139" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140" s="4">
         <f t="shared" si="4"/>
         <v>138</v>
@@ -4710,8 +5556,14 @@
       <c r="I140" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:9">
+      <c r="J140" s="4">
+        <v>2</v>
+      </c>
+      <c r="K140" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141" s="4">
         <f t="shared" si="4"/>
         <v>139</v>
@@ -4739,6 +5591,12 @@
       </c>
       <c r="I141" s="4">
         <v>0</v>
+      </c>
+      <c r="J141" s="4">
+        <v>2</v>
+      </c>
+      <c r="K141" s="11">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -4750,15 +5608,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3A6AB7-4833-A94B-94C3-4DB3EA4569E2}">
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4786,8 +5648,14 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>-1</v>
       </c>
@@ -4807,8 +5675,14 @@
       <c r="I2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -4836,8 +5710,14 @@
       <c r="I3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -4865,8 +5745,14 @@
       <c r="I4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -4894,8 +5780,14 @@
       <c r="I5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -4923,8 +5815,14 @@
       <c r="I6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -4952,8 +5850,14 @@
       <c r="I7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -4981,8 +5885,14 @@
       <c r="I8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -5010,8 +5920,14 @@
       <c r="I9" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -5039,8 +5955,14 @@
       <c r="I10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="4">
         <v>8</v>
       </c>
@@ -5068,8 +5990,14 @@
       <c r="I11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -5097,8 +6025,14 @@
       <c r="I12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="4">
         <v>10</v>
       </c>
@@ -5126,8 +6060,14 @@
       <c r="I13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -5155,8 +6095,14 @@
       <c r="I14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="4">
+        <v>2</v>
+      </c>
+      <c r="K14" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -5184,8 +6130,14 @@
       <c r="I15" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="4">
+        <v>2</v>
+      </c>
+      <c r="K15" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -5213,8 +6165,14 @@
       <c r="I16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="4">
+        <v>2</v>
+      </c>
+      <c r="K16" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -5242,8 +6200,14 @@
       <c r="I17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="4">
         <v>15</v>
       </c>
@@ -5271,8 +6235,14 @@
       <c r="I18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+      <c r="K18" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="4">
         <v>16</v>
       </c>
@@ -5300,8 +6270,14 @@
       <c r="I19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="4">
+        <v>2</v>
+      </c>
+      <c r="K19" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -5329,8 +6305,14 @@
       <c r="I20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="4">
         <v>18</v>
       </c>
@@ -5358,8 +6340,14 @@
       <c r="I21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="4">
+        <v>1</v>
+      </c>
+      <c r="K21" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -5387,8 +6375,14 @@
       <c r="I22" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
+      <c r="K22" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="4">
         <v>20</v>
       </c>
@@ -5416,8 +6410,14 @@
       <c r="I23" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
+      <c r="K23" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -5445,8 +6445,14 @@
       <c r="I24" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="4">
+        <v>1</v>
+      </c>
+      <c r="K24" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="4">
         <v>22</v>
       </c>
@@ -5474,8 +6480,14 @@
       <c r="I25" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="4">
+        <v>1</v>
+      </c>
+      <c r="K25" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="4">
         <v>23</v>
       </c>
@@ -5503,8 +6515,14 @@
       <c r="I26" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="4">
+        <v>1</v>
+      </c>
+      <c r="K26" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="4">
         <v>24</v>
       </c>
@@ -5532,8 +6550,14 @@
       <c r="I27" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="4">
+        <v>1</v>
+      </c>
+      <c r="K27" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -5561,8 +6585,14 @@
       <c r="I28" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="4">
+        <v>2</v>
+      </c>
+      <c r="K28" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="4">
         <f>A28+1</f>
         <v>26</v>
@@ -5591,8 +6621,14 @@
       <c r="I29" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="4">
+        <v>2</v>
+      </c>
+      <c r="K29" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="4">
         <f t="shared" ref="A30:A93" si="0">A29+1</f>
         <v>27</v>
@@ -5621,8 +6657,14 @@
       <c r="I30" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="4">
+        <v>2</v>
+      </c>
+      <c r="K30" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5651,8 +6693,14 @@
       <c r="I31" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="4">
+        <v>2</v>
+      </c>
+      <c r="K31" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -5681,8 +6729,14 @@
       <c r="I32" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="4">
+        <v>2</v>
+      </c>
+      <c r="K32" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5711,8 +6765,14 @@
       <c r="I33" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="4">
+        <v>2</v>
+      </c>
+      <c r="K33" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5741,8 +6801,14 @@
       <c r="I34" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="4">
+        <v>2</v>
+      </c>
+      <c r="K34" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="4">
         <f>A34+1</f>
         <v>32</v>
@@ -5771,8 +6837,14 @@
       <c r="I35" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="4">
+        <v>2</v>
+      </c>
+      <c r="K35" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="4">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -5801,8 +6873,14 @@
       <c r="I36" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="4">
+        <v>2</v>
+      </c>
+      <c r="K36" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -5831,8 +6909,14 @@
       <c r="I37" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="4">
+        <v>2</v>
+      </c>
+      <c r="K37" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -5861,8 +6945,14 @@
       <c r="I38" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="4">
+        <v>2</v>
+      </c>
+      <c r="K38" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -5891,8 +6981,14 @@
       <c r="I39" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="4">
+        <v>2</v>
+      </c>
+      <c r="K39" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="4">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -5921,8 +7017,14 @@
       <c r="I40" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="4">
+        <v>1</v>
+      </c>
+      <c r="K40" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -5951,8 +7053,14 @@
       <c r="I41" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="4">
+        <v>1</v>
+      </c>
+      <c r="K41" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -5981,8 +7089,14 @@
       <c r="I42" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="4">
+        <v>1</v>
+      </c>
+      <c r="K42" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -6011,8 +7125,14 @@
       <c r="I43" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="4">
+        <v>1</v>
+      </c>
+      <c r="K43" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -6041,8 +7161,14 @@
       <c r="I44" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="4">
+        <v>1</v>
+      </c>
+      <c r="K44" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -6071,8 +7197,14 @@
       <c r="I45" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="4">
+        <v>1</v>
+      </c>
+      <c r="K45" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -6101,8 +7233,14 @@
       <c r="I46" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="4">
+        <v>1</v>
+      </c>
+      <c r="K46" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -6131,8 +7269,14 @@
       <c r="I47" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="4">
+        <v>1</v>
+      </c>
+      <c r="K47" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -6161,8 +7305,14 @@
       <c r="I48" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="4">
+        <v>1</v>
+      </c>
+      <c r="K48" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -6191,8 +7341,14 @@
       <c r="I49" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="4">
+        <v>1</v>
+      </c>
+      <c r="K49" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -6221,8 +7377,14 @@
       <c r="I50" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="4">
+        <v>1</v>
+      </c>
+      <c r="K50" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -6251,8 +7413,14 @@
       <c r="I51" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="4">
+        <v>1</v>
+      </c>
+      <c r="K51" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -6281,8 +7449,14 @@
       <c r="I52" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="4">
+        <v>1</v>
+      </c>
+      <c r="K52" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -6311,8 +7485,14 @@
       <c r="I53" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="4">
+        <v>1</v>
+      </c>
+      <c r="K53" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -6341,8 +7521,14 @@
       <c r="I54" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="4">
+        <v>1</v>
+      </c>
+      <c r="K54" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="4">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -6371,8 +7557,14 @@
       <c r="I55" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="4">
+        <v>1</v>
+      </c>
+      <c r="K55" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="4">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -6401,8 +7593,14 @@
       <c r="I56" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="4">
+        <v>1</v>
+      </c>
+      <c r="K56" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="4">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -6431,8 +7629,14 @@
       <c r="I57" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="4">
+        <v>1</v>
+      </c>
+      <c r="K57" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="4">
         <f>A57+1</f>
         <v>55</v>
@@ -6461,8 +7665,14 @@
       <c r="I58" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="4">
+        <v>2</v>
+      </c>
+      <c r="K58" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="4">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -6491,8 +7701,14 @@
       <c r="I59" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" s="4">
+        <v>2</v>
+      </c>
+      <c r="K59" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="4">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -6521,8 +7737,14 @@
       <c r="I60" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" s="4">
+        <v>2</v>
+      </c>
+      <c r="K60" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="4">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -6551,8 +7773,14 @@
       <c r="I61" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" s="4">
+        <v>2</v>
+      </c>
+      <c r="K61" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="4">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -6581,8 +7809,14 @@
       <c r="I62" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" s="4">
+        <v>2</v>
+      </c>
+      <c r="K62" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -6611,8 +7845,14 @@
       <c r="I63" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" s="4">
+        <v>2</v>
+      </c>
+      <c r="K63" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="4">
         <f>A63+1</f>
         <v>61</v>
@@ -6641,8 +7881,14 @@
       <c r="I64" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" s="4">
+        <v>1</v>
+      </c>
+      <c r="K64" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="4">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -6671,8 +7917,14 @@
       <c r="I65" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" s="4">
+        <v>1</v>
+      </c>
+      <c r="K65" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="4">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -6701,8 +7953,14 @@
       <c r="I66" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="J66" s="4">
+        <v>1</v>
+      </c>
+      <c r="K66" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -6731,8 +7989,14 @@
       <c r="I67" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" s="4">
+        <v>2</v>
+      </c>
+      <c r="K67" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="4">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -6761,8 +8025,14 @@
       <c r="I68" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="J68" s="4">
+        <v>2</v>
+      </c>
+      <c r="K68" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="4">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -6791,8 +8061,14 @@
       <c r="I69" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="J69" s="4">
+        <v>2</v>
+      </c>
+      <c r="K69" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="4">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -6821,8 +8097,14 @@
       <c r="I70" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="J70" s="4">
+        <v>2</v>
+      </c>
+      <c r="K70" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="4">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -6851,8 +8133,14 @@
       <c r="I71" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="J71" s="4">
+        <v>2</v>
+      </c>
+      <c r="K71" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="4">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -6881,8 +8169,14 @@
       <c r="I72" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="J72" s="4">
+        <v>2</v>
+      </c>
+      <c r="K72" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="4">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -6911,8 +8205,14 @@
       <c r="I73" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="J73" s="4">
+        <v>2</v>
+      </c>
+      <c r="K73" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="4">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -6941,8 +8241,14 @@
       <c r="I74" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="J74" s="4">
+        <v>2</v>
+      </c>
+      <c r="K74" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="4">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -6971,8 +8277,14 @@
       <c r="I75" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="J75" s="4">
+        <v>2</v>
+      </c>
+      <c r="K75" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="4">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -7001,8 +8313,14 @@
       <c r="I76" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="J76" s="4">
+        <v>2</v>
+      </c>
+      <c r="K76" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="4">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -7031,8 +8349,14 @@
       <c r="I77" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="J77" s="4">
+        <v>2</v>
+      </c>
+      <c r="K77" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="4">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -7061,8 +8385,14 @@
       <c r="I78" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="J78" s="4">
+        <v>2</v>
+      </c>
+      <c r="K78" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="4">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -7091,8 +8421,14 @@
       <c r="I79" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="J79" s="4">
+        <v>2</v>
+      </c>
+      <c r="K79" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="4">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -7121,8 +8457,14 @@
       <c r="I80" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="J80" s="4">
+        <v>2</v>
+      </c>
+      <c r="K80" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="4">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -7151,8 +8493,14 @@
       <c r="I81" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="J81" s="4">
+        <v>1</v>
+      </c>
+      <c r="K81" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="4">
         <f>A81+1</f>
         <v>79</v>
@@ -7181,8 +8529,14 @@
       <c r="I82" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="J82" s="4">
+        <v>1</v>
+      </c>
+      <c r="K82" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="4">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -7211,8 +8565,14 @@
       <c r="I83" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="J83" s="4">
+        <v>1</v>
+      </c>
+      <c r="K83" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="4">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -7241,8 +8601,14 @@
       <c r="I84" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="J84" s="4">
+        <v>1</v>
+      </c>
+      <c r="K84" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="4">
         <f t="shared" si="0"/>
         <v>82</v>
@@ -7271,8 +8637,14 @@
       <c r="I85" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="J85" s="4">
+        <v>1</v>
+      </c>
+      <c r="K85" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="4">
         <f t="shared" si="0"/>
         <v>83</v>
@@ -7301,8 +8673,14 @@
       <c r="I86" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="J86" s="4">
+        <v>1</v>
+      </c>
+      <c r="K86" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="4">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -7331,8 +8709,14 @@
       <c r="I87" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="J87" s="4">
+        <v>1</v>
+      </c>
+      <c r="K87" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="4">
         <f>A87+1</f>
         <v>85</v>
@@ -7361,8 +8745,14 @@
       <c r="I88" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="J88" s="4">
+        <v>1</v>
+      </c>
+      <c r="K88" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" s="4">
         <f t="shared" si="0"/>
         <v>86</v>
@@ -7391,8 +8781,14 @@
       <c r="I89" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="J89" s="4">
+        <v>1</v>
+      </c>
+      <c r="K89" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="4">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -7421,8 +8817,14 @@
       <c r="I90" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="J90" s="4">
+        <v>1</v>
+      </c>
+      <c r="K90" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="4">
         <f t="shared" si="0"/>
         <v>88</v>
@@ -7451,8 +8853,14 @@
       <c r="I91" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="J91" s="4">
+        <v>1</v>
+      </c>
+      <c r="K91" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="4">
         <f t="shared" si="0"/>
         <v>89</v>
@@ -7481,8 +8889,14 @@
       <c r="I92" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="J92" s="4">
+        <v>1</v>
+      </c>
+      <c r="K92" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="4">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -7511,8 +8925,14 @@
       <c r="I93" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="J93" s="4">
+        <v>1</v>
+      </c>
+      <c r="K93" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="4">
         <f t="shared" ref="A94" si="1">A93+1</f>
         <v>91</v>
@@ -7541,8 +8961,14 @@
       <c r="I94" s="5">
         <v>56</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="J94" s="4">
+        <v>1</v>
+      </c>
+      <c r="K94" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="4">
         <f>A94+1</f>
         <v>92</v>
@@ -7571,8 +8997,14 @@
       <c r="I95" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="J95" s="4">
+        <v>1</v>
+      </c>
+      <c r="K95" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="4">
         <f t="shared" ref="A96:A116" si="2">A95+1</f>
         <v>93</v>
@@ -7601,8 +9033,14 @@
       <c r="I96" s="5">
         <v>58</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96" s="4">
+        <v>1</v>
+      </c>
+      <c r="K96" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="4">
         <f t="shared" si="2"/>
         <v>94</v>
@@ -7631,8 +9069,14 @@
       <c r="I97" s="5">
         <v>59</v>
       </c>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="J97" s="4">
+        <v>1</v>
+      </c>
+      <c r="K97" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="4">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -7661,8 +9105,14 @@
       <c r="I98" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="J98" s="4">
+        <v>1</v>
+      </c>
+      <c r="K98" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" s="4">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -7691,8 +9141,14 @@
       <c r="I99" s="5">
         <v>61</v>
       </c>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="J99" s="4">
+        <v>2</v>
+      </c>
+      <c r="K99" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" s="4">
         <f t="shared" si="2"/>
         <v>97</v>
@@ -7721,8 +9177,14 @@
       <c r="I100" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="J100" s="4">
+        <v>2</v>
+      </c>
+      <c r="K100" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" s="4">
         <f>A100+1</f>
         <v>98</v>
@@ -7751,8 +9213,14 @@
       <c r="I101" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="J101" s="4">
+        <v>2</v>
+      </c>
+      <c r="K101" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" s="4">
         <f t="shared" si="2"/>
         <v>99</v>
@@ -7781,8 +9249,14 @@
       <c r="I102" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="J102" s="4">
+        <v>2</v>
+      </c>
+      <c r="K102" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" s="4">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -7811,8 +9285,14 @@
       <c r="I103" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:9">
+      <c r="J103" s="4">
+        <v>2</v>
+      </c>
+      <c r="K103" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" s="4">
         <f t="shared" si="2"/>
         <v>101</v>
@@ -7841,8 +9321,14 @@
       <c r="I104" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="J104" s="4">
+        <v>2</v>
+      </c>
+      <c r="K104" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="4">
         <f t="shared" si="2"/>
         <v>102</v>
@@ -7871,8 +9357,14 @@
       <c r="I105" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="J105" s="4">
+        <v>2</v>
+      </c>
+      <c r="K105" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" s="4">
         <f t="shared" si="2"/>
         <v>103</v>
@@ -7901,8 +9393,14 @@
       <c r="I106" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106" s="4">
+        <v>2</v>
+      </c>
+      <c r="K106" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" s="4">
         <f t="shared" si="2"/>
         <v>104</v>
@@ -7931,8 +9429,14 @@
       <c r="I107" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="J107" s="4">
+        <v>2</v>
+      </c>
+      <c r="K107" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="4">
         <f t="shared" si="2"/>
         <v>105</v>
@@ -7961,8 +9465,14 @@
       <c r="I108" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="J108" s="4">
+        <v>2</v>
+      </c>
+      <c r="K108" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" s="4">
         <f t="shared" si="2"/>
         <v>106</v>
@@ -7991,8 +9501,14 @@
       <c r="I109" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="J109" s="4">
+        <v>2</v>
+      </c>
+      <c r="K109" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" s="4">
         <f t="shared" si="2"/>
         <v>107</v>
@@ -8021,8 +9537,14 @@
       <c r="I110" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="J110" s="4">
+        <v>2</v>
+      </c>
+      <c r="K110" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" s="4">
         <f t="shared" si="2"/>
         <v>108</v>
@@ -8051,8 +9573,14 @@
       <c r="I111" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="J111" s="4">
+        <v>2</v>
+      </c>
+      <c r="K111" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" s="4">
         <f t="shared" si="2"/>
         <v>109</v>
@@ -8081,8 +9609,14 @@
       <c r="I112" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112" s="4">
+        <v>2</v>
+      </c>
+      <c r="K112" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" s="4">
         <f t="shared" si="2"/>
         <v>110</v>
@@ -8111,8 +9645,14 @@
       <c r="I113" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113" s="4">
+        <v>2</v>
+      </c>
+      <c r="K113" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" s="4">
         <f t="shared" si="2"/>
         <v>111</v>
@@ -8141,8 +9681,14 @@
       <c r="I114" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" s="4">
+        <v>2</v>
+      </c>
+      <c r="K114" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" s="4">
         <f t="shared" si="2"/>
         <v>112</v>
@@ -8171,8 +9717,14 @@
       <c r="I115" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115" s="4">
+        <v>2</v>
+      </c>
+      <c r="K115" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" s="4">
         <f t="shared" si="2"/>
         <v>113</v>
@@ -8201,8 +9753,14 @@
       <c r="I116" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116" s="4">
+        <v>1</v>
+      </c>
+      <c r="K116" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" s="4">
         <f>A116+1</f>
         <v>114</v>
@@ -8231,8 +9789,14 @@
       <c r="I117" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="J117" s="4">
+        <v>1</v>
+      </c>
+      <c r="K117" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" s="4">
         <f t="shared" ref="A118:A129" si="3">A117+1</f>
         <v>115</v>
@@ -8261,8 +9825,14 @@
       <c r="I118" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="J118" s="4">
+        <v>1</v>
+      </c>
+      <c r="K118" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" s="4">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -8291,8 +9861,14 @@
       <c r="I119" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="J119" s="4">
+        <v>1</v>
+      </c>
+      <c r="K119" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" s="4">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -8321,8 +9897,14 @@
       <c r="I120" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="J120" s="4">
+        <v>1</v>
+      </c>
+      <c r="K120" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" s="4">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -8351,8 +9933,14 @@
       <c r="I121" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="J121" s="4">
+        <v>1</v>
+      </c>
+      <c r="K121" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" s="4">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -8381,8 +9969,14 @@
       <c r="I122" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="J122" s="4">
+        <v>1</v>
+      </c>
+      <c r="K122" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" s="4">
         <f>A122+1</f>
         <v>120</v>
@@ -8411,8 +10005,14 @@
       <c r="I123" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="J123" s="4">
+        <v>1</v>
+      </c>
+      <c r="K123" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" s="4">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -8441,8 +10041,14 @@
       <c r="I124" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="J124" s="4">
+        <v>1</v>
+      </c>
+      <c r="K124" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" s="4">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -8471,8 +10077,14 @@
       <c r="I125" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="J125" s="4">
+        <v>1</v>
+      </c>
+      <c r="K125" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" s="4">
         <f t="shared" si="3"/>
         <v>123</v>
@@ -8501,8 +10113,14 @@
       <c r="I126" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="J126" s="4">
+        <v>1</v>
+      </c>
+      <c r="K126" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" s="4">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -8531,8 +10149,14 @@
       <c r="I127" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:9">
+      <c r="J127" s="4">
+        <v>1</v>
+      </c>
+      <c r="K127" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" s="4">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -8561,8 +10185,14 @@
       <c r="I128" s="5">
         <v>97</v>
       </c>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="J128" s="4">
+        <v>1</v>
+      </c>
+      <c r="K128" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129" s="4">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -8591,8 +10221,14 @@
       <c r="I129" s="5">
         <v>98</v>
       </c>
-    </row>
-    <row r="130" spans="1:9">
+      <c r="J129" s="4">
+        <v>1</v>
+      </c>
+      <c r="K129" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130" s="4">
         <f>A129+1</f>
         <v>127</v>
@@ -8621,8 +10257,14 @@
       <c r="I130" s="5">
         <v>99</v>
       </c>
-    </row>
-    <row r="131" spans="1:9">
+      <c r="J130" s="4">
+        <v>1</v>
+      </c>
+      <c r="K130" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
       <c r="A131" s="4">
         <f t="shared" ref="A131:A142" si="4">A130+1</f>
         <v>128</v>
@@ -8651,8 +10293,14 @@
       <c r="I131" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="132" spans="1:9">
+      <c r="J131" s="4">
+        <v>2</v>
+      </c>
+      <c r="K131" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
       <c r="A132" s="4">
         <f t="shared" si="4"/>
         <v>129</v>
@@ -8681,8 +10329,14 @@
       <c r="I132" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:9">
+      <c r="J132" s="4">
+        <v>2</v>
+      </c>
+      <c r="K132" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
       <c r="A133" s="4">
         <f t="shared" si="4"/>
         <v>130</v>
@@ -8711,8 +10365,14 @@
       <c r="I133" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:9">
+      <c r="J133" s="4">
+        <v>2</v>
+      </c>
+      <c r="K133" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134" s="4">
         <f t="shared" si="4"/>
         <v>131</v>
@@ -8741,8 +10401,14 @@
       <c r="I134" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:9">
+      <c r="J134" s="4">
+        <v>2</v>
+      </c>
+      <c r="K134" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135" s="4">
         <f t="shared" si="4"/>
         <v>132</v>
@@ -8771,8 +10437,14 @@
       <c r="I135" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:9">
+      <c r="J135" s="4">
+        <v>2</v>
+      </c>
+      <c r="K135" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136" s="4">
         <f>A135+1</f>
         <v>133</v>
@@ -8801,8 +10473,14 @@
       <c r="I136" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:9">
+      <c r="J136" s="4">
+        <v>2</v>
+      </c>
+      <c r="K136" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137" s="4">
         <f t="shared" si="4"/>
         <v>134</v>
@@ -8831,8 +10509,14 @@
       <c r="I137" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="J137" s="4">
+        <v>2</v>
+      </c>
+      <c r="K137" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" s="4">
         <f t="shared" si="4"/>
         <v>135</v>
@@ -8861,8 +10545,14 @@
       <c r="I138" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:9">
+      <c r="J138" s="4">
+        <v>2</v>
+      </c>
+      <c r="K138" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" s="4">
         <f t="shared" si="4"/>
         <v>136</v>
@@ -8891,8 +10581,14 @@
       <c r="I139" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:9">
+      <c r="J139" s="4">
+        <v>2</v>
+      </c>
+      <c r="K139" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140" s="4">
         <f t="shared" si="4"/>
         <v>137</v>
@@ -8921,8 +10617,14 @@
       <c r="I140" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:9">
+      <c r="J140" s="4">
+        <v>2</v>
+      </c>
+      <c r="K140" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141" s="4">
         <f t="shared" si="4"/>
         <v>138</v>
@@ -8951,8 +10653,14 @@
       <c r="I141" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:9">
+      <c r="J141" s="4">
+        <v>2</v>
+      </c>
+      <c r="K141" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
       <c r="A142" s="4">
         <f t="shared" si="4"/>
         <v>139</v>

</xml_diff>